<commit_message>
Project Tower Motor Rater is saved. Fixed null issue Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Tower Motor Rater/PMT,CMT,MTB-rules-01012017-01012017.xlsx
+++ b/DESIGN/rules/Tower Motor Rater/PMT,CMT,MTB-rules-01012017-01012017.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="1283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="1287">
   <si>
     <t>Environment</t>
   </si>
@@ -5740,6 +5740,18 @@
   </si>
   <si>
     <t>Updated multiplicative rules, NCB, SI factor, Windscreen rate</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>= isEmpty (result) ? $initial : addWithoutNulls (result, $first )</t>
+  </si>
+  <si>
+    <t>Spreadsheet OptionalCoverage[][] combine ( OptionalCoverage[][] covs, OptionalCoverage[][] result )</t>
+  </si>
+  <si>
+    <t>calculateAllCells</t>
   </si>
 </sst>
 </file>
@@ -6058,7 +6070,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.34998626667073579" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6145,7 +6157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -6606,7 +6618,7 @@
         <color theme="0" tint="-0.14996795556505021"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.14996795556505021" rgb="FFFFFF"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14996795556505021"/>
@@ -6619,7 +6631,7 @@
       </left>
       <right/>
       <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.14996795556505021" rgb="FFFFFF"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14996795556505021"/>
@@ -6649,7 +6661,7 @@
         <color theme="0" tint="-0.14996795556505021"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.14996795556505021" rgb="FFFFFF"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -6668,7 +6680,7 @@
         <color theme="0" tint="-0.14996795556505021"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.14996795556505021" rgb="FFFFFF"/>
       </right>
       <top/>
       <bottom/>
@@ -6679,7 +6691,7 @@
         <color theme="0" tint="-0.14996795556505021"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="0" tint="-0.14996795556505021" rgb="FFFFFF"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -6756,8 +6768,22 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="3" tint="0.39994506668294322"/>
+        <color theme="3" tint="0.39994506668294322" rgb="1F497D"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -6783,9 +6809,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="53"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="489">
+  <cellXfs count="509">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8079,6 +8105,26 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name=" 1" xfId="3"/>
@@ -13831,7 +13877,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO177"/>
+  <dimension ref="A1:AA177"/>
   <sheetViews>
     <sheetView topLeftCell="C23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
@@ -13839,41 +13885,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="29.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="185.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="46" style="3" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="77.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="43.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="68.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15" customWidth="1" collapsed="1"/>
-    <col min="26" max="27" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="28" max="29" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="15" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="35" max="37" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="15" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="13" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="29.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="185.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="46.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="3" width="77.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="3" width="43.140625" collapsed="true"/>
+    <col min="8" max="9" bestFit="true" customWidth="true" width="68.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="26" max="27" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="28" max="29" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="35" max="37" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="82" customFormat="1" x14ac:dyDescent="0.25">
@@ -16516,10 +16562,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="50" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="48.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="50.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="48.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -16643,10 +16689,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="120.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="67.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="76.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="42.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="120.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="67.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="76.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -17871,7 +17917,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I25"/>
+  <dimension ref="B3:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
@@ -17879,14 +17925,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="251"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="40.140625" customWidth="1"/>
-    <col min="9" max="9" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" style="251" width="9.140625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="26.28515625" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="20.5703125" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="19.7109375" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="40.140625" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="38.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -18238,7 +18284,7 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="C1:G47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C24" sqref="C24:D24"/>
@@ -18246,10 +18292,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="82" collapsed="1"/>
-    <col min="3" max="3" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="84.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" style="82" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="84.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:6" s="82" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18581,12 +18627,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="47.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="47.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="31.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -18997,10 +19043,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="106.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="66.42578125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="106.42578125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="41.140625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="16.28515625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:4" s="251" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -19814,83 +19860,89 @@
     </row>
     <row r="131" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C131" s="411" t="s">
-        <v>814</v>
+        <v>1285</v>
       </c>
       <c r="D131" s="411"/>
-      <c r="E131" s="216"/>
+      <c r="E131" s="508"/>
       <c r="F131" s="216"/>
       <c r="G131" s="216"/>
     </row>
     <row r="132" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C132" s="200" t="s">
-        <v>558</v>
-      </c>
-      <c r="D132" s="219" t="s">
-        <v>254</v>
-      </c>
-      <c r="E132" s="216"/>
+      <c r="C132" s="489" t="s">
+        <v>820</v>
+      </c>
+      <c r="D132" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E132" s="491" t="b">
+        <v>0</v>
+      </c>
       <c r="F132" s="216"/>
       <c r="G132" s="216"/>
     </row>
     <row r="133" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C133" s="201" t="s">
-        <v>561</v>
-      </c>
-      <c r="D133" s="220" t="s">
-        <v>560</v>
-      </c>
-      <c r="E133" s="216"/>
+      <c r="C133" s="200" t="s">
+        <v>558</v>
+      </c>
+      <c r="D133" s="219" t="s">
+        <v>254</v>
+      </c>
+      <c r="E133" s="497"/>
       <c r="F133" s="216"/>
       <c r="G133" s="216"/>
     </row>
     <row r="134" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C134" s="201" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D134" s="220" t="s">
-        <v>563</v>
-      </c>
-      <c r="E134" s="216"/>
+        <v>560</v>
+      </c>
+      <c r="E134" s="498"/>
       <c r="F134" s="216"/>
       <c r="G134" s="216"/>
     </row>
     <row r="135" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C135" s="201" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D135" s="220" t="s">
-        <v>568</v>
-      </c>
-      <c r="E135" s="216"/>
+        <v>563</v>
+      </c>
+      <c r="E135" s="499"/>
       <c r="F135" s="216"/>
       <c r="G135" s="216"/>
     </row>
     <row r="136" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C136" s="201" t="s">
-        <v>564</v>
-      </c>
-      <c r="D136" s="255" t="s">
-        <v>816</v>
-      </c>
-      <c r="E136" s="216"/>
+        <v>565</v>
+      </c>
+      <c r="D136" s="220" t="s">
+        <v>568</v>
+      </c>
+      <c r="E136" s="500"/>
       <c r="F136" s="216"/>
       <c r="G136" s="216"/>
     </row>
     <row r="137" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C137" s="205" t="s">
-        <v>24</v>
-      </c>
-      <c r="D137" s="204" t="s">
-        <v>566</v>
-      </c>
-      <c r="E137" s="216"/>
+      <c r="C137" s="201" t="s">
+        <v>564</v>
+      </c>
+      <c r="D137" s="255" t="s">
+        <v>1284</v>
+      </c>
+      <c r="E137" s="501"/>
       <c r="F137" s="216"/>
       <c r="G137" s="216"/>
     </row>
     <row r="138" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C138" s="216"/>
-      <c r="D138" s="216"/>
-      <c r="E138" s="216"/>
+      <c r="C138" s="205" t="s">
+        <v>24</v>
+      </c>
+      <c r="D138" s="204" t="s">
+        <v>566</v>
+      </c>
+      <c r="E138" s="502"/>
       <c r="F138" s="216"/>
       <c r="G138" s="216"/>
     </row>
@@ -19956,12 +20008,18 @@
     <mergeCell ref="C113:D113"/>
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C131:D131"/>
     <mergeCell ref="C141:D141"/>
     <mergeCell ref="C120:D120"/>
     <mergeCell ref="C122:C123"/>
     <mergeCell ref="C124:C127"/>
     <mergeCell ref="D125:D127"/>
+    <mergeCell ref="C131:E131"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -19976,8 +20034,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="40.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
@@ -20012,10 +20070,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="74.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="74.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -20860,19 +20918,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" style="10" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.140625" style="10" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" style="10" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="94.5703125" style="10" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="47.7109375" style="10" customWidth="1" collapsed="1"/>
-    <col min="6" max="10" width="21.28515625" style="10" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.42578125" style="10" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.42578125" style="10" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="9.140625" style="10" collapsed="1"/>
-    <col min="16" max="16" width="30" style="10" customWidth="1" collapsed="1"/>
-    <col min="17" max="18" width="9.140625" style="10" collapsed="1"/>
-    <col min="19" max="19" width="23.5703125" style="10" customWidth="1" collapsed="1"/>
-    <col min="20" max="16384" width="9.140625" style="10" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="10" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" style="10" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="10" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="10" width="94.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="10" width="47.7109375" collapsed="true"/>
+    <col min="6" max="10" customWidth="true" style="10" width="21.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="10" width="17.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="10" width="23.42578125" collapsed="true"/>
+    <col min="13" max="15" style="10" width="9.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="10" width="30.0" collapsed="true"/>
+    <col min="17" max="18" style="10" width="9.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="10" width="23.5703125" collapsed="true"/>
+    <col min="20" max="16384" style="10" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="202" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -22323,9 +22381,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="77" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30.140625" style="50" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="77.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="50" width="30.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -23399,9 +23457,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="53.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="79.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="79.5703125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:5" s="162" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -23887,7 +23945,7 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="B1:G45"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
@@ -23895,11 +23953,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="82" collapsed="1"/>
-    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="147.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="72.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="71.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="82" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="147.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="72.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="71.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:7" s="82" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -24305,10 +24363,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="54.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="96.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="54.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="96.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.7109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
@@ -24587,7 +24645,7 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A1:Y506"/>
+  <dimension ref="A1:K506"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
@@ -24595,26 +24653,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="64.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="48.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="39.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="56" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="29.28515625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="39.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="34.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="64.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="48.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="39.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="34.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:4" s="82" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -31215,11 +31273,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="89.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="59.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="89.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:6" s="251" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -31489,7 +31547,7 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="A2:S92"/>
+  <dimension ref="C2:S92"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C21" sqref="C21:D21"/>
@@ -31497,15 +31555,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="50" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="56" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="49.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="50" width="17.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="49.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="9" max="10" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:19" x14ac:dyDescent="0.25">

</xml_diff>